<commit_message>
some notes and further mutations
</commit_message>
<xml_diff>
--- a/tweede_kamer/tweede_kamer_mutations.xlsx
+++ b/tweede_kamer/tweede_kamer_mutations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmuenchow/Desktop/work/tweede_kamer/C7-Subproject-GER-NED/tweede_kamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29BDBF0E-D1F6-9445-B1F9-7927DA75D8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A30AE3F-59BE-384D-89BC-F14274436C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="1980" windowWidth="13740" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="13740" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Article (roman)</t>
   </si>
@@ -172,6 +172,48 @@
   </si>
   <si>
     <t>in onderdeel P</t>
+  </si>
+  <si>
+    <t>artikel 32bb</t>
+  </si>
+  <si>
+    <t>artikel 3.92b</t>
+  </si>
+  <si>
+    <t>artikel 32bc</t>
+  </si>
+  <si>
+    <t>onderdeel b</t>
+  </si>
+  <si>
+    <t>In hetderde lid (ACHTUNG: leerzeichen fehlt)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">punt twee </t>
+  </si>
+  <si>
+    <t>subonderdeel</t>
+  </si>
+  <si>
+    <t>subonderdeel 2</t>
+  </si>
+  <si>
+    <t>van artikel 9a</t>
+  </si>
+  <si>
+    <t>Onderdeel B</t>
+  </si>
+  <si>
+    <t>Onderdeel b</t>
+  </si>
+  <si>
+    <t>artikelen I tot en met III</t>
+  </si>
+  <si>
+    <t>onder 2 (?) (59)</t>
+  </si>
+  <si>
+    <t>Note: until amends[60]</t>
   </si>
 </sst>
 </file>
@@ -532,22 +574,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D238DB4-537C-CC4E-826F-9CE6670785FD}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="30.5" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="3" width="30.5" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,42 +597,45 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -598,16 +643,25 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -615,115 +669,153 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
         <v>39</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>44</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
       <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="E9" t="s">
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="E10" t="s">
+      <c r="D10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E11" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E12" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E13" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E14" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E15" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E16" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E18" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E20" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented further mutations of articles;
</commit_message>
<xml_diff>
--- a/tweede_kamer/tweede_kamer_mutations.xlsx
+++ b/tweede_kamer/tweede_kamer_mutations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmuenchow/Desktop/work/tweede_kamer/C7-Subproject-GER-NED/tweede_kamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A30AE3F-59BE-384D-89BC-F14274436C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A11A4A-6FE2-5E44-AD80-8A2DA8AB3664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="13740" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
+    <workbookView xWindow="11640" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>Article (roman)</t>
   </si>
@@ -213,7 +213,22 @@
     <t>onder 2 (?) (59)</t>
   </si>
   <si>
-    <t>Note: until amends[60]</t>
+    <t>voor onderdeel A</t>
+  </si>
+  <si>
+    <t>Artikel 44</t>
+  </si>
+  <si>
+    <t>Artikel 8.14a</t>
+  </si>
+  <si>
+    <t>artikel 8.9</t>
+  </si>
+  <si>
+    <t>artikel 9a</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -237,12 +252,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -257,9 +284,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,7 +606,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,7 +665,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
@@ -645,7 +674,7 @@
       <c r="C5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
@@ -662,7 +691,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
@@ -671,7 +700,7 @@
       <c r="C6" t="s">
         <v>58</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>39</v>
       </c>
       <c r="E6" t="s">
@@ -682,13 +711,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>40</v>
       </c>
       <c r="E7" t="s">
@@ -699,13 +728,13 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E8" t="s">
@@ -716,13 +745,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>46</v>
       </c>
       <c r="F9" t="s">
@@ -733,7 +762,7 @@
       <c r="B10" t="s">
         <v>45</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>47</v>
       </c>
       <c r="F10" t="s">
@@ -744,7 +773,7 @@
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
       <c r="F11" t="s">
@@ -755,7 +784,7 @@
       <c r="B12" t="s">
         <v>55</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>54</v>
       </c>
       <c r="F12" t="s">
@@ -766,54 +795,69 @@
       <c r="B13" t="s">
         <v>56</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="F13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="F14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="F15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D16" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="F16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>64</v>
+      </c>
       <c r="F20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
identify onderdeel + collapsing of list elements + further mutations
</commit_message>
<xml_diff>
--- a/tweede_kamer/tweede_kamer_mutations.xlsx
+++ b/tweede_kamer/tweede_kamer_mutations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmuenchow/Desktop/work/tweede_kamer/C7-Subproject-GER-NED/tweede_kamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A11A4A-6FE2-5E44-AD80-8A2DA8AB3664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829936E-0757-B943-BCC6-7249CE90049B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11640" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
+    <workbookView xWindow="6280" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
   <si>
     <t>Article (roman)</t>
   </si>
@@ -120,9 +120,6 @@
     <t>onderdelen a en b</t>
   </si>
   <si>
-    <t>twee onderdelen (ACHTUNG: nur ein e)</t>
-  </si>
-  <si>
     <t>na het eerste lid</t>
   </si>
   <si>
@@ -228,7 +225,28 @@
     <t>artikel 9a</t>
   </si>
   <si>
-    <t>s</t>
+    <t xml:space="preserve">onderdelen A en B </t>
+  </si>
+  <si>
+    <t>lid 2</t>
+  </si>
+  <si>
+    <t>lid 3</t>
+  </si>
+  <si>
+    <t>deerde punt</t>
+  </si>
+  <si>
+    <t>Punt één tot en met punt 4</t>
+  </si>
+  <si>
+    <t>vierde onderdeel</t>
+  </si>
+  <si>
+    <t>onderdeel BW</t>
+  </si>
+  <si>
+    <t>sub b</t>
   </si>
 </sst>
 </file>
@@ -284,11 +302,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -603,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D238DB4-537C-CC4E-826F-9CE6670785FD}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,7 +633,7 @@
     <col min="1" max="1" width="23.1640625" customWidth="1"/>
     <col min="2" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="24" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,7 +645,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -638,10 +657,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -658,53 +677,53 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
         <v>41</v>
-      </c>
-      <c r="C6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -714,14 +733,14 @@
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>28</v>
+      <c r="C7" t="s">
+        <v>70</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -731,14 +750,14 @@
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -746,120 +765,142 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
+        <v>56</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>45</v>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>49</v>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>55</v>
+      <c r="B12" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>56</v>
+      <c r="B13" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>59</v>
+      <c r="B14" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>68</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
         <v>64</v>
       </c>
-      <c r="F20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="F22" t="s">
-        <v>50</v>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mutations for onderdeel, punt and lid; Cleaning of action text
</commit_message>
<xml_diff>
--- a/tweede_kamer/tweede_kamer_mutations.xlsx
+++ b/tweede_kamer/tweede_kamer_mutations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmuenchow/Desktop/work/tweede_kamer/C7-Subproject-GER-NED/tweede_kamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A829936E-0757-B943-BCC6-7249CE90049B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573DED92-BFA7-FB4B-A191-14A3F6A2B7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6280" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>Article (roman)</t>
   </si>
@@ -162,9 +162,6 @@
     <t>het tweede punt</t>
   </si>
   <si>
-    <t>het eerste punt</t>
-  </si>
-  <si>
     <t>punt 4</t>
   </si>
   <si>
@@ -247,6 +244,15 @@
   </si>
   <si>
     <t>sub b</t>
+  </si>
+  <si>
+    <t>tweede tot en met achtste lid</t>
+  </si>
+  <si>
+    <t>negende tot tiende lid</t>
+  </si>
+  <si>
+    <t>eerste punt</t>
   </si>
 </sst>
 </file>
@@ -622,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D238DB4-537C-CC4E-826F-9CE6670785FD}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,6 +640,7 @@
     <col min="2" max="3" width="30.5" customWidth="1"/>
     <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -645,7 +652,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -691,15 +698,15 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
@@ -717,15 +724,15 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -734,15 +741,15 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -757,150 +764,160 @@
         <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="F16" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F18" t="s">
+      <c r="F18" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F21" t="s">
+      <c r="F21" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F22" t="s">
-        <v>49</v>
+      <c r="F22" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F23" t="s">
+      <c r="F23" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F24" t="s">
-        <v>65</v>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="F26" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
text.spec + text.cite + adjustment for introductory sentence
</commit_message>
<xml_diff>
--- a/tweede_kamer/tweede_kamer_mutations.xlsx
+++ b/tweede_kamer/tweede_kamer_mutations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmuenchow/Desktop/work/tweede_kamer/C7-Subproject-GER-NED/tweede_kamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D213F9E2-A32D-5142-AB6A-7D8405CC5030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D52C6A9-04BB-5742-843D-B3EEAC9615AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6280" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -631,7 +632,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
aanhef + fix for text.cite
</commit_message>
<xml_diff>
--- a/tweede_kamer/tweede_kamer_mutations.xlsx
+++ b/tweede_kamer/tweede_kamer_mutations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmuenchow/Desktop/work/tweede_kamer/C7-Subproject-GER-NED/tweede_kamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D52C6A9-04BB-5742-843D-B3EEAC9615AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090D6831-4D08-3241-A1B6-3FDDFF634E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6280" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -632,7 +631,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -710,7 +709,7 @@
       <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H5" t="s">

</xml_diff>

<commit_message>
made action_matrix more compatible
</commit_message>
<xml_diff>
--- a/tweede_kamer/tweede_kamer_mutations.xlsx
+++ b/tweede_kamer/tweede_kamer_mutations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felixmuenchow/Desktop/work/tweede_kamer/C7-Subproject-GER-NED/tweede_kamer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090D6831-4D08-3241-A1B6-3FDDFF634E3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00181FBE-E089-1A4E-836C-DDB594C9B5D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
+    <workbookView xWindow="15340" yWindow="460" windowWidth="22520" windowHeight="16660" xr2:uid="{8882561E-CAAE-5543-AD4F-E6F153B8C4F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -308,12 +308,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -631,7 +632,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -712,7 +713,7 @@
       <c r="G5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="5" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>